<commit_message>
Updated Plantilla Factura y BBDD
</commit_message>
<xml_diff>
--- a/templates/plantilla_factura.xlsx
+++ b/templates/plantilla_factura.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AUTOMATIZACION\FACTURAS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Extintores el Tumi\OneDrive\Escritorio\AUTOMATIZACION NUEVO\crm-backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4813D1D7-93BA-4EEC-9E5C-283BAB6FFD47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75848C97-6DFB-43FC-A06C-03CEBBB390A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1350,7 +1350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I960"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
@@ -1363,7 +1363,7 @@
     <col min="5" max="5" width="9.7109375" style="4" customWidth="1"/>
     <col min="6" max="6" width="43.140625" style="4" customWidth="1"/>
     <col min="7" max="7" width="8.28515625" style="4" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" style="4" customWidth="1"/>
     <col min="9" max="21" width="10" style="4" customWidth="1"/>
     <col min="22" max="16384" width="14.42578125" style="4"/>
   </cols>

</xml_diff>